<commit_message>
Add 2025 emissions target
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_ZeroCO2_2050_Tougher.xlsx
+++ b/SuppXLS/Scen_SYS_ZeroCO2_2050_Tougher.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37F836F-BD56-41AB-BA19-B5D364F064E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A37CA7-4B78-408C-8EBC-966D5BC0A6C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -58,7 +58,7 @@
     <author>tc={D7F7A51F-98CC-4BD8-BF17-ABDD25DA4C1B}</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{D7F7A51F-98CC-4BD8-BF17-ABDD25DA4C1B}">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{D7F7A51F-98CC-4BD8-BF17-ABDD25DA4C1B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="89">
   <si>
     <t>LimType</t>
   </si>
@@ -1147,7 +1147,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C7" dT="2021-03-03T22:33:41.43" personId="{1B80334F-2539-4DC6-A837-54D1ADCF10B1}" id="{D7F7A51F-98CC-4BD8-BF17-ABDD25DA4C1B}">
+  <threadedComment ref="D7" dT="2021-03-03T22:33:41.43" personId="{1B80334F-2539-4DC6-A837-54D1ADCF10B1}" id="{D7F7A51F-98CC-4BD8-BF17-ABDD25DA4C1B}">
     <text>i.e. &gt;60% reduction from the 2018 value (ca. 40 Mt based on https://www.epa.ie/pubs/reports/air/airemissions/ghg2018/Ireland%20GHG%201990-2018%20Final%20Inventory_April%202020.pdf )</text>
   </threadedComment>
 </ThreadedComments>
@@ -1922,25 +1922,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F14" sqref="C14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="12" width="9.140625" style="8"/>
+    <col min="3" max="3" width="21.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.140625" style="8"/>
     <col min="13" max="13" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="B1"/>
       <c r="C1"/>
@@ -1959,7 +1959,7 @@
       <c r="P1"/>
       <c r="Q1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1978,7 +1978,7 @@
       <c r="P2"/>
       <c r="Q2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
@@ -1997,7 +1997,7 @@
       <c r="P3"/>
       <c r="Q3"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" t="s">
         <v>61</v>
@@ -2020,7 +2020,7 @@
       <c r="P4"/>
       <c r="Q4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" t="s">
         <v>66</v>
@@ -2043,84 +2043,110 @@
       <c r="P5"/>
       <c r="Q5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C6" s="8">
+        <v>2025</v>
+      </c>
+      <c r="D6" s="8">
         <v>2030</v>
       </c>
-      <c r="D6" s="8">
+      <c r="E6" s="8">
         <v>2050</v>
       </c>
-      <c r="E6" s="8">
+      <c r="F6" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="8">
-        <v>15000</v>
+        <v>28095</v>
       </c>
       <c r="D7" s="8">
+        <v>15724</v>
+      </c>
+      <c r="E7" s="8">
         <v>0</v>
       </c>
-      <c r="E7" s="8">
+      <c r="F7" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>77</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D8" s="8" t="str">
+        <f>C8</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="E8" s="8" t="str">
+        <f>D8</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>62</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D9" s="8" t="str">
+        <f t="shared" ref="D9:E9" si="0">C9</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="E9" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>71</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D10" s="8" t="str">
+        <f t="shared" ref="D10:E12" si="1">C10</f>
+        <v>ENV</v>
+      </c>
+      <c r="E10" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>ENV</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D12" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>UP</v>
+      </c>
+      <c r="E12" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>UP</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>85</v>
       </c>
@@ -2128,21 +2154,30 @@
         <v>-1</v>
       </c>
       <c r="D13" s="8">
+        <f t="shared" ref="D13:E13" si="2">C13</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E13" s="8">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14" t="s">
         <v>86</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="8">
         <v>1</v>
       </c>
       <c r="D14" s="8">
+        <f t="shared" ref="D14:E14" si="3">C14</f>
         <v>1</v>
       </c>
-      <c r="E14"/>
+      <c r="E14" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
@@ -2155,8 +2190,9 @@
       <c r="O14"/>
       <c r="P14"/>
       <c r="Q14"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -2175,7 +2211,7 @@
       <c r="P15"/>
       <c r="Q15"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -2222,10 +2258,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9318C9B-7F0A-410C-BCB5-F22D93E1F454}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2316,115 +2352,163 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B$5, config!$B$4:$E$14,2,FALSE) &amp; "_Single"</f>
+        <f>VLOOKUP(B$5, config!$B$4:$F$14,2,FALSE) &amp; "_Single"</f>
         <v>UC_NetZero_CO2_2050_Single</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F7" s="8">
-        <f>VLOOKUP(F$5, config!$B$4:$E$14,2,FALSE)</f>
-        <v>2030</v>
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,2,FALSE)</f>
+        <v>2025</v>
       </c>
       <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H7" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$E$14,2,FALSE)</f>
-        <v>15000</v>
+        <f>VLOOKUP("Value", config!$B$4:$F$14,2,FALSE)</f>
+        <v>28095</v>
       </c>
       <c r="K7" s="8" t="str">
-        <f>VLOOKUP(K$5, config!$B$4:$E$14,2,FALSE) &amp; " - Single"</f>
+        <f>VLOOKUP(K$5, config!$B$4:$F$14,2,FALSE) &amp; " - Single"</f>
         <v>Net Zero CO2 by 2050 - Single</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E8" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F8" s="8">
-        <f>VLOOKUP(F$5, config!$B$4:$E$14,2,FALSE)</f>
-        <v>2030</v>
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,2,FALSE)</f>
+        <v>2025</v>
       </c>
       <c r="I8" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F9" s="8">
-        <f>VLOOKUP(F$5, config!$B$4:$E$14,3,FALSE)</f>
-        <v>2050</v>
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,3,FALSE)</f>
+        <v>2030</v>
       </c>
       <c r="G9" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H9" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J9" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$E$14,3,FALSE)</f>
-        <v>0</v>
+        <f>VLOOKUP("Value", config!$B$4:$F$14,3,FALSE)</f>
+        <v>15724</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E10" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F10" s="8">
-        <f>VLOOKUP(F$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,3,FALSE)</f>
+        <v>2030</v>
+      </c>
+      <c r="I10" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$F$14,3,FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D11" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F11" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,4,FALSE)</f>
         <v>2050</v>
       </c>
-      <c r="I10" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$E$14,3,FALSE)</f>
+      <c r="G11" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H11" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J11" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$F$14,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D12" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E12" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F12" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>2050</v>
+      </c>
+      <c r="I12" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$F$14,4,FALSE)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F11" s="8">
-        <f>VLOOKUP(F$5, config!$B$4:$E$14,4,FALSE)</f>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,5,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$E$14,4,FALSE)</f>
+      <c r="J13" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$F$14,5,FALSE)</f>
         <v>5</v>
       </c>
     </row>
@@ -2436,10 +2520,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,115 +2614,163 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B$5, config!$B$4:$E$14,2,FALSE) &amp; "_Multi"</f>
+        <f>VLOOKUP(B$5, config!$B$4:$F$14,2,FALSE) &amp; "_Multi"</f>
         <v>UC_NetZero_CO2_2050_Multi</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F7" s="8">
-        <f>VLOOKUP(F$5, config!$B$4:$E$14,2,FALSE)</f>
-        <v>2030</v>
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,2,FALSE)</f>
+        <v>2025</v>
       </c>
       <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H7" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$E$14,2,FALSE)</f>
-        <v>15000</v>
+        <f>VLOOKUP("Value", config!$B$4:$F$14,2,FALSE)</f>
+        <v>28095</v>
       </c>
       <c r="K7" s="8" t="str">
-        <f>VLOOKUP(K$5, config!$B$4:$E$14,2,FALSE) &amp; " - Multi"</f>
+        <f>VLOOKUP(K$5, config!$B$4:$F$14,2,FALSE) &amp; " - Multi"</f>
         <v>Net Zero CO2 by 2050 - Multi</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E8" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F8" s="8">
-        <f>VLOOKUP(F$5, config!$B$4:$E$14,2,FALSE)</f>
-        <v>2030</v>
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,2,FALSE)</f>
+        <v>2025</v>
       </c>
       <c r="I8" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$E$14,2,FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F9" s="8">
-        <f>VLOOKUP(F$5, config!$B$4:$E$14,3,FALSE)</f>
-        <v>2050</v>
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,3,FALSE)</f>
+        <v>2030</v>
       </c>
       <c r="G9" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H9" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>1</v>
       </c>
       <c r="J9" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$E$14,3,FALSE)</f>
-        <v>0</v>
+        <f>VLOOKUP("Value", config!$B$4:$F$14,3,FALSE)</f>
+        <v>15724</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E10" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F10" s="8">
-        <f>VLOOKUP(F$5, config!$B$4:$E$14,3,FALSE)</f>
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,3,FALSE)</f>
+        <v>2030</v>
+      </c>
+      <c r="I10" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$F$14,3,FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D11" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F11" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,4,FALSE)</f>
         <v>2050</v>
       </c>
-      <c r="I10" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$E$14,3,FALSE)</f>
+      <c r="G11" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H11" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J11" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$F$14,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D12" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E12" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F12" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,4,FALSE)</f>
+        <v>2050</v>
+      </c>
+      <c r="I12" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$F$14,4,FALSE)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F11" s="8">
-        <f>VLOOKUP(F$5, config!$B$4:$E$14,4,FALSE)</f>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$F$14,5,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$E$14,4,FALSE)</f>
+      <c r="J13" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$F$14,5,FALSE)</f>
         <v>5</v>
       </c>
     </row>

</xml_diff>